<commit_message>
Add blank worksheets within excel-test*.xls* for testing purposes.
</commit_message>
<xml_diff>
--- a/Blueprints/Tests/excel-test2.xlsx
+++ b/Blueprints/Tests/excel-test2.xlsx
@@ -1,22 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="330" windowWidth="28515" windowHeight="12045"/>
+    <workbookView xWindow="240" yWindow="330" windowWidth="28515" windowHeight="12045" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2 (2)" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet2 (3)" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet2 (4)" sheetId="6" r:id="rId6"/>
+    <sheet name="LastOne" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="5">
   <si>
     <t>d</t>
   </si>
@@ -25,6 +29,12 @@
   </si>
   <si>
     <t>#dig Excel testing</t>
+  </si>
+  <si>
+    <t>#dig Excel testing sheet last</t>
+  </si>
+  <si>
+    <t>#dig Excel testing sheet in middle</t>
   </si>
 </sst>
 </file>
@@ -356,32 +366,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.140625" defaultRowHeight="17.25" customHeight="1"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="17.25" customHeight="1">
+    <row r="1" spans="1:7" ht="17.25" customHeight="1">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="17.25" customHeight="1">
-      <c r="D2" t="s">
+    <row r="2" spans="1:7" ht="17.25" customHeight="1">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="E2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="17.25" customHeight="1">
-      <c r="C3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" t="s">
+    <row r="3" spans="1:7" ht="17.25" customHeight="1">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -413,4 +433,126 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="4.140625" defaultRowHeight="17.25" customHeight="1"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="17.25" customHeight="1">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="17.25" customHeight="1">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="17.25" customHeight="1">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="4.140625" defaultRowHeight="17.25" customHeight="1"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="17.25" customHeight="1">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="17.25" customHeight="1">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="17.25" customHeight="1">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>